<commit_message>
Finished reviewing & revising all results
</commit_message>
<xml_diff>
--- a/data/imputed/Congressional Election Results by State (2002 - 108th) UNCONTESTED.xlsx
+++ b/data/imputed/Congressional Election Results by State (2002 - 108th) UNCONTESTED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/ushouse/data/imputed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25E4221E-A7D0-C84E-BC19-C41B95888B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FEE809-298C-E846-9751-63303FFD328F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1000" windowWidth="26860" windowHeight="16440" xr2:uid="{A6D7AFE9-EF1A-994E-9F8C-B9D930E51A69}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="Congressional_Election_Results_by_State__2002___108th__UNCONTESTED" localSheetId="0">Sheet1!$A$1:$F$107</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{FD8CD97A-1460-9D44-8F7D-0332E72DA5A2}" name="Congressional Election Results by State (2002 - 108th) UNCONTESTED" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/alecramsay/Documents/dev/ushouse/data/imputed/Congressional Election Results by State (2002 - 108th) UNCONTESTED.csv" comma="1">
+    <textPr sourceFile="/Users/alecramsay/Documents/dev/ushouse/data/imputed/Congressional Election Results by State (2002 - 108th) UNCONTESTED.csv" comma="1">
       <textFields count="6">
         <textField type="text"/>
         <textField type="text"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="119">
   <si>
     <t>STATE</t>
   </si>
@@ -374,6 +374,45 @@
   </si>
   <si>
     <t>WY</t>
+  </si>
+  <si>
+    <t>5th</t>
+  </si>
+  <si>
+    <t>6th</t>
+  </si>
+  <si>
+    <t>10th</t>
+  </si>
+  <si>
+    <t>12th</t>
+  </si>
+  <si>
+    <t>18th</t>
+  </si>
+  <si>
+    <t>23rd</t>
+  </si>
+  <si>
+    <t>24th</t>
+  </si>
+  <si>
+    <t>DISTRICT</t>
+  </si>
+  <si>
+    <t>REP_S</t>
+  </si>
+  <si>
+    <t>DEM_S</t>
+  </si>
+  <si>
+    <t>OTH_S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Recast (implied)</t>
   </si>
 </sst>
 </file>
@@ -397,12 +436,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -417,13 +462,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,13 +790,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C40DF2D-D61E-A244-8122-36E072635518}">
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:T107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="Q62" sqref="Q62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,6 +806,8 @@
     <col min="3" max="4" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" customWidth="1"/>
+    <col min="16" max="16" width="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1720,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -1740,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -1760,7 +1810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
@@ -1780,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>58</v>
       </c>
@@ -1800,7 +1850,7 @@
         <v>34175</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
@@ -1820,7 +1870,7 @@
         <v>58243</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>60</v>
       </c>
@@ -1840,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>62</v>
       </c>
@@ -1860,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>64</v>
       </c>
@@ -1879,8 +1929,11 @@
       <c r="F56" s="2">
         <v>42677</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="Q56" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>66</v>
       </c>
@@ -1899,28 +1952,108 @@
       <c r="F57" s="2">
         <v>52680</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+      <c r="H57" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K57" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L57" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M57" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="N57" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="O57" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q57" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R57" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="S57" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="T57" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="7">
         <v>63968</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="7">
         <v>48218</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58" s="7">
         <v>-63968</v>
       </c>
-      <c r="F58" s="2">
+      <c r="F58" s="7">
         <v>48218</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="I58" s="8">
+        <v>0</v>
+      </c>
+      <c r="J58" s="8">
+        <v>68773</v>
+      </c>
+      <c r="K58" s="8">
+        <v>63968</v>
+      </c>
+      <c r="L58" s="8">
+        <v>132741</v>
+      </c>
+      <c r="M58" s="8">
+        <v>0</v>
+      </c>
+      <c r="N58" s="8">
+        <v>1</v>
+      </c>
+      <c r="O58" s="8">
+        <v>0</v>
+      </c>
+      <c r="P58" s="8"/>
+      <c r="Q58" s="7">
+        <f>I58+C58</f>
+        <v>63968</v>
+      </c>
+      <c r="R58" s="7">
+        <f t="shared" ref="R58:T58" si="0">J58+D58</f>
+        <v>116991</v>
+      </c>
+      <c r="S58" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T58" s="7">
+        <f t="shared" si="0"/>
+        <v>180959</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>68</v>
       </c>
@@ -1939,8 +2072,51 @@
       <c r="F59" s="2">
         <v>55312</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59" t="s">
+        <v>117</v>
+      </c>
+      <c r="H59" t="s">
+        <v>107</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>68718</v>
+      </c>
+      <c r="K59">
+        <v>43100</v>
+      </c>
+      <c r="L59">
+        <v>111818</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>1</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="2">
+        <f t="shared" ref="Q59:Q64" si="1">I59+C59</f>
+        <v>50139</v>
+      </c>
+      <c r="R59" s="2">
+        <f t="shared" ref="R59:R64" si="2">J59+D59</f>
+        <v>116991</v>
+      </c>
+      <c r="S59" s="2">
+        <f t="shared" ref="S59:S64" si="3">K59+E59</f>
+        <v>0</v>
+      </c>
+      <c r="T59" s="2">
+        <f t="shared" ref="T59:T64" si="4">L59+F59</f>
+        <v>167130</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>68</v>
       </c>
@@ -1959,8 +2135,51 @@
       <c r="F60" s="2">
         <v>49559</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60" t="s">
+        <v>117</v>
+      </c>
+      <c r="H60" t="s">
+        <v>108</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>72313</v>
+      </c>
+      <c r="K60">
+        <v>45258</v>
+      </c>
+      <c r="L60">
+        <v>117571</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>1</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="2">
+        <f t="shared" si="1"/>
+        <v>50139</v>
+      </c>
+      <c r="R60" s="2">
+        <f t="shared" si="2"/>
+        <v>116991</v>
+      </c>
+      <c r="S60" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T60" s="2">
+        <f t="shared" si="4"/>
+        <v>167130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>68</v>
       </c>
@@ -1979,48 +2198,179 @@
       <c r="F61" s="2">
         <v>82365</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+      <c r="G61" t="s">
+        <v>117</v>
+      </c>
+      <c r="H61" t="s">
+        <v>109</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>43809</v>
+      </c>
+      <c r="K61">
+        <v>40956</v>
+      </c>
+      <c r="L61">
+        <v>84765</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>1</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="2">
+        <f t="shared" si="1"/>
+        <v>50139</v>
+      </c>
+      <c r="R61" s="2">
+        <f t="shared" si="2"/>
+        <v>116991</v>
+      </c>
+      <c r="S61" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T61" s="2">
+        <f t="shared" si="4"/>
+        <v>167130</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="7">
         <v>94622</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="7">
         <v>21595</v>
       </c>
-      <c r="E62" s="2">
+      <c r="E62" s="7">
         <v>-94622</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F62" s="7">
         <v>21595</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+      <c r="G62" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I62" s="8">
+        <v>0</v>
+      </c>
+      <c r="J62" s="8">
+        <v>95396</v>
+      </c>
+      <c r="K62" s="8">
+        <v>94622</v>
+      </c>
+      <c r="L62" s="8">
+        <v>190018</v>
+      </c>
+      <c r="M62" s="8">
+        <v>0</v>
+      </c>
+      <c r="N62" s="8">
+        <v>1</v>
+      </c>
+      <c r="O62" s="8">
+        <v>0</v>
+      </c>
+      <c r="P62" s="8"/>
+      <c r="Q62" s="7">
+        <f t="shared" si="1"/>
+        <v>94622</v>
+      </c>
+      <c r="R62" s="7">
+        <f t="shared" si="2"/>
+        <v>116991</v>
+      </c>
+      <c r="S62" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T62" s="7">
+        <f t="shared" si="4"/>
+        <v>211613</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="7">
         <v>6949</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="7">
         <v>74571</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63" s="7">
         <v>-74571</v>
       </c>
-      <c r="F63" s="2">
+      <c r="F63" s="7">
         <v>6949</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H63" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="I63" s="8">
+        <v>110042</v>
+      </c>
+      <c r="J63" s="8">
+        <v>0</v>
+      </c>
+      <c r="K63" s="8">
+        <v>74571</v>
+      </c>
+      <c r="L63" s="8">
+        <v>184613</v>
+      </c>
+      <c r="M63" s="8">
+        <v>1</v>
+      </c>
+      <c r="N63" s="8">
+        <v>0</v>
+      </c>
+      <c r="O63" s="8">
+        <v>0</v>
+      </c>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="7">
+        <f t="shared" si="1"/>
+        <v>116991</v>
+      </c>
+      <c r="R63" s="7">
+        <f t="shared" si="2"/>
+        <v>74571</v>
+      </c>
+      <c r="S63" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T63" s="7">
+        <f t="shared" si="4"/>
+        <v>191562</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>68</v>
       </c>
@@ -2038,6 +2388,49 @@
       </c>
       <c r="F64" s="2">
         <v>8974</v>
+      </c>
+      <c r="G64" t="s">
+        <v>117</v>
+      </c>
+      <c r="H64" t="s">
+        <v>112</v>
+      </c>
+      <c r="I64">
+        <v>108017</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>94615</v>
+      </c>
+      <c r="L64">
+        <v>202632</v>
+      </c>
+      <c r="M64">
+        <v>1</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="2">
+        <f t="shared" si="1"/>
+        <v>116991</v>
+      </c>
+      <c r="R64" s="2">
+        <f t="shared" si="2"/>
+        <v>94615</v>
+      </c>
+      <c r="S64" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T64" s="2">
+        <f t="shared" si="4"/>
+        <v>211606</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>